<commit_message>
New Course Outline is being prepared
</commit_message>
<xml_diff>
--- a/FALL 2020/CSE 480/team_dist_cse480_sec1.xlsx
+++ b/FALL 2020/CSE 480/team_dist_cse480_sec1.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ulab_course_materials\FALL 2020\CSE 480\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F89702B0-C357-4089-9A62-6B965A1D1E90}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A805C55B-5958-48B4-AB48-47EB8A6A4DD7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="4">
   <si>
     <t>Name</t>
   </si>
@@ -39,78 +39,6 @@
   </si>
   <si>
     <t>Code</t>
-  </si>
-  <si>
-    <t>Anika Tahsin Sababa</t>
-  </si>
-  <si>
-    <t>Mahbubur Rahman</t>
-  </si>
-  <si>
-    <t>Swarnali Dey</t>
-  </si>
-  <si>
-    <t>Nuzhat Farhana Prekkha</t>
-  </si>
-  <si>
-    <t>Fahmeda Gulzar</t>
-  </si>
-  <si>
-    <t>Mahabub Rahman</t>
-  </si>
-  <si>
-    <t>Asifa Sultana</t>
-  </si>
-  <si>
-    <t>Aldrin Abir Halder</t>
-  </si>
-  <si>
-    <t>Gibson Modhu Eric</t>
-  </si>
-  <si>
-    <t>Fahim Afroz Tasnimul Haque</t>
-  </si>
-  <si>
-    <t>Shahnila Mahbub</t>
-  </si>
-  <si>
-    <t>Sadia Hasan</t>
-  </si>
-  <si>
-    <t>A.S.M Arafat Kamal</t>
-  </si>
-  <si>
-    <t>Md. Mahmudur Rahman</t>
-  </si>
-  <si>
-    <t>Md. Abdul kamrun Faisal</t>
-  </si>
-  <si>
-    <t>Salma Sayeeda Orpa</t>
-  </si>
-  <si>
-    <t>Md. Muhtasim Fuad Fahim</t>
-  </si>
-  <si>
-    <t>Anika Nusrat Ridme</t>
-  </si>
-  <si>
-    <t>Ayon Mazumder</t>
-  </si>
-  <si>
-    <t>Sabiha Sumaiya</t>
-  </si>
-  <si>
-    <t>Md. Ashikur Rahaman</t>
-  </si>
-  <si>
-    <t>Tabachsum Islam</t>
-  </si>
-  <si>
-    <t>Tamanna Islam</t>
-  </si>
-  <si>
-    <t>Prianka Uddin</t>
   </si>
 </sst>
 </file>
@@ -555,8 +483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -585,76 +513,68 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2">
+      <c r="A2" s="12"/>
+      <c r="B2" t="e">
         <f>VLOOKUP(A2,Sheet2!$A$2:$B$30,2,FALSE)</f>
-        <v>153014016</v>
+        <v>#N/A</v>
       </c>
       <c r="C2">
         <v>5</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="e">
         <f>B2</f>
-        <v>153014016</v>
+        <v>#N/A</v>
       </c>
       <c r="E2">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3">
+      <c r="A3" s="12"/>
+      <c r="B3" t="e">
         <f>VLOOKUP(A3,Sheet2!$A$2:$B$30,2,FALSE)</f>
-        <v>172014016</v>
+        <v>#N/A</v>
       </c>
       <c r="C3">
         <v>5</v>
       </c>
-      <c r="D3">
+      <c r="D3" t="e">
         <f t="shared" ref="D3:D5" si="0">B3</f>
-        <v>172014016</v>
+        <v>#N/A</v>
       </c>
       <c r="E3">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4">
+      <c r="A4" s="12"/>
+      <c r="B4" t="e">
         <f>VLOOKUP(A4,Sheet2!$A$2:$B$30,2,FALSE)</f>
-        <v>171014006</v>
+        <v>#N/A</v>
       </c>
       <c r="C4">
         <v>4.5</v>
       </c>
-      <c r="D4">
-        <f t="shared" si="0"/>
-        <v>171014006</v>
+      <c r="D4" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
       </c>
       <c r="E4">
         <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5">
+      <c r="A5" s="12"/>
+      <c r="B5" t="e">
         <f>VLOOKUP(A5,Sheet2!$A$2:$B$30,2,FALSE)</f>
-        <v>153014015</v>
+        <v>#N/A</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>153014015</v>
+      <c r="D5" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
       </c>
       <c r="E5">
         <v>19</v>
@@ -664,76 +584,68 @@
       <c r="A6" s="11"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7">
+      <c r="A7" s="12"/>
+      <c r="B7" t="e">
         <f>VLOOKUP(A7,Sheet2!$A$2:$B$30,2,FALSE)</f>
-        <v>172014007</v>
+        <v>#N/A</v>
       </c>
       <c r="C7">
         <v>5</v>
       </c>
-      <c r="D7">
+      <c r="D7" t="e">
         <f>B7</f>
-        <v>172014007</v>
+        <v>#N/A</v>
       </c>
       <c r="E7">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8">
+      <c r="A8" s="12"/>
+      <c r="B8" t="e">
         <f>VLOOKUP(A8,Sheet2!$A$2:$B$30,2,FALSE)</f>
-        <v>171011166</v>
+        <v>#N/A</v>
       </c>
       <c r="C8">
         <v>4</v>
       </c>
-      <c r="D8">
+      <c r="D8" t="e">
         <f t="shared" ref="D8:D10" si="1">B8</f>
-        <v>171011166</v>
+        <v>#N/A</v>
       </c>
       <c r="E8">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9">
+      <c r="A9" s="12"/>
+      <c r="B9" t="e">
         <f>VLOOKUP(A9,Sheet2!$A$2:$B$30,2,FALSE)</f>
-        <v>172014052</v>
+        <v>#N/A</v>
       </c>
       <c r="C9">
         <v>4</v>
       </c>
-      <c r="D9">
+      <c r="D9" t="e">
         <f t="shared" si="1"/>
-        <v>172014052</v>
+        <v>#N/A</v>
       </c>
       <c r="E9">
         <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10">
+      <c r="A10" s="12"/>
+      <c r="B10" t="e">
         <f>VLOOKUP(A10,Sheet2!$A$2:$B$30,2,FALSE)</f>
-        <v>172014051</v>
+        <v>#N/A</v>
       </c>
       <c r="C10">
         <v>4</v>
       </c>
-      <c r="D10">
+      <c r="D10" t="e">
         <f t="shared" si="1"/>
-        <v>172014051</v>
+        <v>#N/A</v>
       </c>
       <c r="E10">
         <v>18</v>
@@ -743,76 +655,68 @@
       <c r="A11" s="11"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12">
+      <c r="A12" s="12"/>
+      <c r="B12" t="e">
         <f>VLOOKUP(A12,Sheet2!$A$2:$B$30,2,FALSE)</f>
-        <v>143014008</v>
+        <v>#N/A</v>
       </c>
       <c r="C12">
         <v>4.5</v>
       </c>
-      <c r="D12">
+      <c r="D12" t="e">
         <f>B12</f>
-        <v>143014008</v>
+        <v>#N/A</v>
       </c>
       <c r="E12">
         <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13">
+      <c r="A13" s="12"/>
+      <c r="B13" t="e">
         <f>VLOOKUP(A13,Sheet2!$A$2:$B$30,2,FALSE)</f>
-        <v>171014032</v>
+        <v>#N/A</v>
       </c>
       <c r="C13">
         <v>4.5</v>
       </c>
-      <c r="D13">
+      <c r="D13" t="e">
         <f t="shared" ref="D13:D15" si="2">B13</f>
-        <v>171014032</v>
+        <v>#N/A</v>
       </c>
       <c r="E13">
         <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14">
+      <c r="A14" s="12"/>
+      <c r="B14" t="e">
         <f>VLOOKUP(A14,Sheet2!$A$2:$B$30,2,FALSE)</f>
-        <v>151014002</v>
+        <v>#N/A</v>
       </c>
       <c r="C14">
         <v>4.5</v>
       </c>
-      <c r="D14">
+      <c r="D14" t="e">
         <f t="shared" si="2"/>
-        <v>151014002</v>
+        <v>#N/A</v>
       </c>
       <c r="E14">
         <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15">
+      <c r="A15" s="12"/>
+      <c r="B15" t="e">
         <f>VLOOKUP(A15,Sheet2!$A$2:$B$30,2,FALSE)</f>
-        <v>161014019</v>
+        <v>#N/A</v>
       </c>
       <c r="C15">
         <v>4.5</v>
       </c>
-      <c r="D15">
+      <c r="D15" t="e">
         <f t="shared" si="2"/>
-        <v>161014019</v>
+        <v>#N/A</v>
       </c>
       <c r="E15">
         <v>17</v>
@@ -822,76 +726,68 @@
       <c r="A16" s="11"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17">
+      <c r="A17" s="12"/>
+      <c r="B17" t="e">
         <f>VLOOKUP(A17,Sheet2!$A$2:$B$30,2,FALSE)</f>
-        <v>163014016</v>
+        <v>#N/A</v>
       </c>
       <c r="C17">
         <v>4.5</v>
       </c>
-      <c r="D17">
+      <c r="D17" t="e">
         <f>B17</f>
-        <v>163014016</v>
+        <v>#N/A</v>
       </c>
       <c r="E17">
         <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18">
+      <c r="A18" s="12"/>
+      <c r="B18" t="e">
         <f>VLOOKUP(A18,Sheet2!$A$2:$B$30,2,FALSE)</f>
-        <v>163014011</v>
+        <v>#N/A</v>
       </c>
       <c r="C18">
         <v>4.5</v>
       </c>
-      <c r="D18">
+      <c r="D18" t="e">
         <f t="shared" ref="D18:D20" si="3">B18</f>
-        <v>163014011</v>
+        <v>#N/A</v>
       </c>
       <c r="E18">
         <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19">
+      <c r="A19" s="12"/>
+      <c r="B19" t="e">
         <f>VLOOKUP(A19,Sheet2!$A$2:$B$30,2,FALSE)</f>
-        <v>171014068</v>
+        <v>#N/A</v>
       </c>
       <c r="C19">
         <v>4.5</v>
       </c>
-      <c r="D19">
+      <c r="D19" t="e">
         <f t="shared" si="3"/>
-        <v>171014068</v>
+        <v>#N/A</v>
       </c>
       <c r="E19">
         <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20">
+      <c r="A20" s="12"/>
+      <c r="B20" t="e">
         <f>VLOOKUP(A20,Sheet2!$A$2:$B$30,2,FALSE)</f>
-        <v>181014110</v>
+        <v>#N/A</v>
       </c>
       <c r="C20">
         <v>4.5</v>
       </c>
-      <c r="D20">
+      <c r="D20" t="e">
         <f t="shared" si="3"/>
-        <v>181014110</v>
+        <v>#N/A</v>
       </c>
       <c r="E20">
         <v>17</v>
@@ -901,76 +797,68 @@
       <c r="A21" s="11"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22">
+      <c r="A22" s="12"/>
+      <c r="B22" t="e">
         <f>VLOOKUP(A22,Sheet2!$A$2:$B$30,2,FALSE)</f>
-        <v>171014075</v>
+        <v>#N/A</v>
       </c>
       <c r="C22">
         <v>5</v>
       </c>
-      <c r="D22">
+      <c r="D22" t="e">
         <f>B22</f>
-        <v>171014075</v>
+        <v>#N/A</v>
       </c>
       <c r="E22">
         <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23">
+      <c r="A23" s="12"/>
+      <c r="B23" t="e">
         <f>VLOOKUP(A23,Sheet2!$A$2:$B$30,2,FALSE)</f>
-        <v>171014012</v>
+        <v>#N/A</v>
       </c>
       <c r="C23">
         <v>5</v>
       </c>
-      <c r="D23">
+      <c r="D23" t="e">
         <f t="shared" ref="D23:D25" si="4">B23</f>
-        <v>171014012</v>
+        <v>#N/A</v>
       </c>
       <c r="E23">
         <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B24">
+      <c r="A24" s="12"/>
+      <c r="B24" t="e">
         <f>VLOOKUP(A24,Sheet2!$A$2:$B$30,2,FALSE)</f>
-        <v>171014022</v>
+        <v>#N/A</v>
       </c>
       <c r="C24">
         <v>4</v>
       </c>
-      <c r="D24">
+      <c r="D24" t="e">
         <f t="shared" si="4"/>
-        <v>171014022</v>
+        <v>#N/A</v>
       </c>
       <c r="E24">
         <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B25">
+      <c r="A25" s="12"/>
+      <c r="B25" t="e">
         <f>VLOOKUP(A25,Sheet2!$A$2:$B$30,2,FALSE)</f>
-        <v>162014022</v>
+        <v>#N/A</v>
       </c>
       <c r="C25">
         <v>4</v>
       </c>
-      <c r="D25">
+      <c r="D25" t="e">
         <f t="shared" si="4"/>
-        <v>162014022</v>
+        <v>#N/A</v>
       </c>
       <c r="E25">
         <v>18</v>
@@ -980,76 +868,68 @@
       <c r="A26" s="11"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B27">
+      <c r="A27" s="12"/>
+      <c r="B27" t="e">
         <f>VLOOKUP(A27,Sheet2!$A$2:$B$30,2,FALSE)</f>
-        <v>171014051</v>
+        <v>#N/A</v>
       </c>
       <c r="C27">
         <v>5</v>
       </c>
-      <c r="D27">
+      <c r="D27" t="e">
         <f>B27</f>
-        <v>171014051</v>
+        <v>#N/A</v>
       </c>
       <c r="E27">
         <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B28">
+      <c r="A28" s="12"/>
+      <c r="B28" t="e">
         <f>VLOOKUP(A28,Sheet2!$A$2:$B$30,2,FALSE)</f>
-        <v>171014048</v>
+        <v>#N/A</v>
       </c>
       <c r="C28">
         <v>0</v>
       </c>
-      <c r="D28">
+      <c r="D28" t="e">
         <f t="shared" ref="D28:D30" si="5">B28</f>
-        <v>171014048</v>
+        <v>#N/A</v>
       </c>
       <c r="E28">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B29">
+      <c r="A29" s="12"/>
+      <c r="B29" t="e">
         <f>VLOOKUP(A29,Sheet2!$A$2:$B$30,2,FALSE)</f>
-        <v>171014037</v>
+        <v>#N/A</v>
       </c>
       <c r="C29">
         <v>4.5</v>
       </c>
-      <c r="D29">
+      <c r="D29" t="e">
         <f t="shared" si="5"/>
-        <v>171014037</v>
+        <v>#N/A</v>
       </c>
       <c r="E29">
         <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B30">
+      <c r="A30" s="12"/>
+      <c r="B30" t="e">
         <f>VLOOKUP(A30,Sheet2!$A$2:$B$30,2,FALSE)</f>
-        <v>171014042</v>
+        <v>#N/A</v>
       </c>
       <c r="C30">
         <v>4</v>
       </c>
-      <c r="D30">
+      <c r="D30" t="e">
         <f t="shared" si="5"/>
-        <v>171014042</v>
+        <v>#N/A</v>
       </c>
       <c r="E30">
         <v>18</v>
@@ -1128,8 +1008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A107198-DDC1-4AB3-9E9C-88DE1D8FD690}">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E25"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1148,312 +1028,248 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="4">
-        <v>171011166</v>
-      </c>
+      <c r="A2" s="5"/>
+      <c r="B2" s="4"/>
       <c r="C2">
         <f>IFERROR(VLOOKUP($B2,Sheet1!$B$2:$C$30,2,FALSE),0)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D2">
         <f>IFERROR(VLOOKUP($B2,Sheet1!$D$2:$E$30,2,FALSE),0)</f>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E2">
         <f>C2+D2</f>
-        <v>24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="4">
-        <v>143014008</v>
-      </c>
+      <c r="A3" s="5"/>
+      <c r="B3" s="4"/>
       <c r="C3">
         <f>IFERROR(VLOOKUP($B3,Sheet1!$B$2:$C$30,2,FALSE),0)</f>
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <f>IFERROR(VLOOKUP($B3,Sheet1!$D$2:$E$30,2,FALSE),0)</f>
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E25" si="0">C3+D3</f>
-        <v>21.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4">
-        <v>151014002</v>
-      </c>
+      <c r="A4" s="5"/>
+      <c r="B4" s="4"/>
       <c r="C4">
         <f>IFERROR(VLOOKUP($B4,Sheet1!$B$2:$C$30,2,FALSE),0)</f>
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <f>IFERROR(VLOOKUP($B4,Sheet1!$D$2:$E$30,2,FALSE),0)</f>
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>21.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="4">
-        <v>153014015</v>
-      </c>
+      <c r="A5" s="5"/>
+      <c r="B5" s="4"/>
       <c r="C5">
         <f>IFERROR(VLOOKUP($B5,Sheet1!$B$2:$C$30,2,FALSE),0)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <f>IFERROR(VLOOKUP($B5,Sheet1!$D$2:$E$30,2,FALSE),0)</f>
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="4">
-        <v>153014016</v>
-      </c>
+      <c r="A6" s="5"/>
+      <c r="B6" s="4"/>
       <c r="C6">
         <f>IFERROR(VLOOKUP($B6,Sheet1!$B$2:$C$30,2,FALSE),0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D6">
         <f>IFERROR(VLOOKUP($B6,Sheet1!$D$2:$E$30,2,FALSE),0)</f>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="4">
-        <v>161014019</v>
-      </c>
+      <c r="A7" s="5"/>
+      <c r="B7" s="4"/>
       <c r="C7">
         <f>IFERROR(VLOOKUP($B7,Sheet1!$B$2:$C$30,2,FALSE),0)</f>
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="D7">
         <f>IFERROR(VLOOKUP($B7,Sheet1!$D$2:$E$30,2,FALSE),0)</f>
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>21.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="4">
-        <v>162014022</v>
-      </c>
+      <c r="A8" s="5"/>
+      <c r="B8" s="4"/>
       <c r="C8">
         <f>IFERROR(VLOOKUP($B8,Sheet1!$B$2:$C$30,2,FALSE),0)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D8">
         <f>IFERROR(VLOOKUP($B8,Sheet1!$D$2:$E$30,2,FALSE),0)</f>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="4">
-        <v>163014011</v>
-      </c>
+      <c r="A9" s="5"/>
+      <c r="B9" s="4"/>
       <c r="C9">
         <f>IFERROR(VLOOKUP($B9,Sheet1!$B$2:$C$30,2,FALSE),0)</f>
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="D9">
         <f>IFERROR(VLOOKUP($B9,Sheet1!$D$2:$E$30,2,FALSE),0)</f>
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>21.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="4">
-        <v>163014016</v>
-      </c>
+      <c r="A10" s="5"/>
+      <c r="B10" s="4"/>
       <c r="C10">
         <f>IFERROR(VLOOKUP($B10,Sheet1!$B$2:$C$30,2,FALSE),0)</f>
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="D10">
         <f>IFERROR(VLOOKUP($B10,Sheet1!$D$2:$E$30,2,FALSE),0)</f>
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>21.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="4">
-        <v>171014006</v>
-      </c>
+      <c r="A11" s="5"/>
+      <c r="B11" s="4"/>
       <c r="C11">
         <f>IFERROR(VLOOKUP($B11,Sheet1!$B$2:$C$30,2,FALSE),0)</f>
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="D11">
         <f>IFERROR(VLOOKUP($B11,Sheet1!$D$2:$E$30,2,FALSE),0)</f>
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>23.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="4">
-        <v>171014012</v>
-      </c>
+      <c r="A12" s="5"/>
+      <c r="B12" s="4"/>
       <c r="C12">
         <f>IFERROR(VLOOKUP($B12,Sheet1!$B$2:$C$30,2,FALSE),0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D12">
         <f>IFERROR(VLOOKUP($B12,Sheet1!$D$2:$E$30,2,FALSE),0)</f>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="4">
-        <v>171014022</v>
-      </c>
+      <c r="A13" s="5"/>
+      <c r="B13" s="4"/>
       <c r="C13">
         <f>IFERROR(VLOOKUP($B13,Sheet1!$B$2:$C$30,2,FALSE),0)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D13">
         <f>IFERROR(VLOOKUP($B13,Sheet1!$D$2:$E$30,2,FALSE),0)</f>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="4">
-        <v>171014032</v>
-      </c>
+      <c r="A14" s="5"/>
+      <c r="B14" s="4"/>
       <c r="C14">
         <f>IFERROR(VLOOKUP($B14,Sheet1!$B$2:$C$30,2,FALSE),0)</f>
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="D14">
         <f>IFERROR(VLOOKUP($B14,Sheet1!$D$2:$E$30,2,FALSE),0)</f>
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>21.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="4">
-        <v>171014037</v>
-      </c>
+      <c r="A15" s="5"/>
+      <c r="B15" s="4"/>
       <c r="C15">
         <f>IFERROR(VLOOKUP($B15,Sheet1!$B$2:$C$30,2,FALSE),0)</f>
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="D15">
         <f>IFERROR(VLOOKUP($B15,Sheet1!$D$2:$E$30,2,FALSE),0)</f>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>22.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="4">
-        <v>171014042</v>
-      </c>
+      <c r="A16" s="5"/>
+      <c r="B16" s="4"/>
       <c r="C16">
         <f>IFERROR(VLOOKUP($B16,Sheet1!$B$2:$C$30,2,FALSE),0)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D16">
         <f>IFERROR(VLOOKUP($B16,Sheet1!$D$2:$E$30,2,FALSE),0)</f>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="E16">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="4">
-        <v>171014048</v>
-      </c>
+      <c r="A17" s="5"/>
+      <c r="B17" s="4"/>
       <c r="C17">
         <f>IFERROR(VLOOKUP($B17,Sheet1!$B$2:$C$30,2,FALSE),0)</f>
         <v>0</v>
@@ -1468,163 +1284,131 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="4">
-        <v>171014051</v>
-      </c>
+      <c r="A18" s="5"/>
+      <c r="B18" s="4"/>
       <c r="C18">
         <f>IFERROR(VLOOKUP($B18,Sheet1!$B$2:$C$30,2,FALSE),0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D18">
         <f>IFERROR(VLOOKUP($B18,Sheet1!$D$2:$E$30,2,FALSE),0)</f>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E18">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="4">
-        <v>171014068</v>
-      </c>
+      <c r="A19" s="5"/>
+      <c r="B19" s="4"/>
       <c r="C19">
         <f>IFERROR(VLOOKUP($B19,Sheet1!$B$2:$C$30,2,FALSE),0)</f>
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="D19">
         <f>IFERROR(VLOOKUP($B19,Sheet1!$D$2:$E$30,2,FALSE),0)</f>
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="E19">
         <f t="shared" si="0"/>
-        <v>21.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="4">
-        <v>171014075</v>
-      </c>
+      <c r="A20" s="5"/>
+      <c r="B20" s="4"/>
       <c r="C20">
         <f>IFERROR(VLOOKUP($B20,Sheet1!$B$2:$C$30,2,FALSE),0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D20">
         <f>IFERROR(VLOOKUP($B20,Sheet1!$D$2:$E$30,2,FALSE),0)</f>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="E20">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" s="4">
-        <v>172014007</v>
-      </c>
+      <c r="A21" s="5"/>
+      <c r="B21" s="4"/>
       <c r="C21">
         <f>IFERROR(VLOOKUP($B21,Sheet1!$B$2:$C$30,2,FALSE),0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D21">
         <f>IFERROR(VLOOKUP($B21,Sheet1!$D$2:$E$30,2,FALSE),0)</f>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E21">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" s="4">
-        <v>172014016</v>
-      </c>
+      <c r="A22" s="5"/>
+      <c r="B22" s="4"/>
       <c r="C22">
         <f>IFERROR(VLOOKUP($B22,Sheet1!$B$2:$C$30,2,FALSE),0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D22">
         <f>IFERROR(VLOOKUP($B22,Sheet1!$D$2:$E$30,2,FALSE),0)</f>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E22">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23" s="4">
-        <v>172014051</v>
-      </c>
+      <c r="A23" s="5"/>
+      <c r="B23" s="4"/>
       <c r="C23">
         <f>IFERROR(VLOOKUP($B23,Sheet1!$B$2:$C$30,2,FALSE),0)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D23">
         <f>IFERROR(VLOOKUP($B23,Sheet1!$D$2:$E$30,2,FALSE),0)</f>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="E23">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" s="4">
-        <v>172014052</v>
-      </c>
+      <c r="A24" s="5"/>
+      <c r="B24" s="4"/>
       <c r="C24">
         <f>IFERROR(VLOOKUP($B24,Sheet1!$B$2:$C$30,2,FALSE),0)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D24">
         <f>IFERROR(VLOOKUP($B24,Sheet1!$D$2:$E$30,2,FALSE),0)</f>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="E24">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25" s="4">
-        <v>181014110</v>
-      </c>
+      <c r="A25" s="5"/>
+      <c r="B25" s="4"/>
       <c r="C25">
         <f>IFERROR(VLOOKUP($B25,Sheet1!$B$2:$C$30,2,FALSE),0)</f>
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="D25">
         <f>IFERROR(VLOOKUP($B25,Sheet1!$D$2:$E$30,2,FALSE),0)</f>
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="E25">
         <f t="shared" si="0"/>
-        <v>21.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>